<commit_message>
add result of FCT&throughput
add FCT and Throughput result
</commit_message>
<xml_diff>
--- a/fct/show.xlsx
+++ b/fct/show.xlsx
@@ -8,21 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\GitHub\line plot draw\Draw-Python-plot\fct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62B8F5E-3412-410B-BE2F-C35BB794A69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BC9084-3B5F-4E11-B49B-D53599B57199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="5">
   <si>
     <t>RC</t>
   </si>
@@ -33,11 +47,11 @@
     <t>ERD</t>
   </si>
   <si>
-    <t>num</t>
+    <t>node</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>X:Server数--Y:FCT</t>
+    <t>FCT(128bit)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -106,6 +120,487 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1200">
+                <a:latin typeface="微软雅黑" pitchFamily="34" charset="-122"/>
+                <a:ea typeface="微软雅黑" pitchFamily="34" charset="-122"/>
+              </a:rPr>
+              <a:t>Server Number</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200">
+              <a:latin typeface="微软雅黑" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" pitchFamily="34" charset="-122"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.38294444444444453"/>
+          <c:y val="0.80555555555555569"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17103018372703419"/>
+          <c:y val="5.3252405949256357E-2"/>
+          <c:w val="0.66656692913385829"/>
+          <c:h val="0.64822506561679805"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$I$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.41</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.61</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.86</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.98</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A488-44D1-BF05-34D2E011C385}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>XRC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$I$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$I$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.63</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.73</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.69</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.5199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.9400000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A488-44D1-BF05-34D2E011C385}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ERD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$I$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.46</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.09</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.97</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.78</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A488-44D1-BF05-34D2E011C385}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="78987264"/>
+        <c:axId val="78988800"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="78987264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="78988800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="78988800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr>
+                    <a:latin typeface="微软雅黑" pitchFamily="34" charset="-122"/>
+                    <a:ea typeface="微软雅黑" pitchFamily="34" charset="-122"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN">
+                    <a:latin typeface="微软雅黑" pitchFamily="34" charset="-122"/>
+                    <a:ea typeface="微软雅黑" pitchFamily="34" charset="-122"/>
+                  </a:rPr>
+                  <a:t>FCT</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" baseline="0">
+                    <a:latin typeface="微软雅黑" pitchFamily="34" charset="-122"/>
+                    <a:ea typeface="微软雅黑" pitchFamily="34" charset="-122"/>
+                  </a:rPr>
+                  <a:t> (MS)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US">
+                  <a:latin typeface="微软雅黑" pitchFamily="34" charset="-122"/>
+                  <a:ea typeface="微软雅黑" pitchFamily="34" charset="-122"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="6.1111111111111116E-2"/>
+              <c:y val="0.25782771945173522"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="78987264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.85426377952755894"/>
+          <c:y val="0.25960921551472732"/>
+          <c:w val="0.12906955380577428"/>
+          <c:h val="0.25115157480314959"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -395,10 +890,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>32</v>
+      </c>
+      <c r="D3">
+        <v>48</v>
+      </c>
+      <c r="E3">
+        <v>64</v>
+      </c>
+      <c r="F3">
+        <v>80</v>
+      </c>
+      <c r="G3">
+        <v>96</v>
+      </c>
+      <c r="H3">
+        <v>112</v>
+      </c>
+      <c r="I3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1.34</v>
+      </c>
+      <c r="C4">
+        <v>3.41</v>
+      </c>
+      <c r="D4">
+        <v>5.61</v>
+      </c>
+      <c r="E4">
+        <v>6.26</v>
+      </c>
+      <c r="F4">
+        <v>6.86</v>
+      </c>
+      <c r="G4">
+        <v>6.98</v>
+      </c>
+      <c r="H4">
+        <v>9.25</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C5">
+        <v>1.63</v>
+      </c>
+      <c r="D5">
+        <v>2.95</v>
+      </c>
+      <c r="E5">
+        <v>4.18</v>
+      </c>
+      <c r="F5">
+        <v>3.73</v>
+      </c>
+      <c r="G5">
+        <v>3.69</v>
+      </c>
+      <c r="H5">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="I5">
+        <v>4.9400000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>0.45</v>
+      </c>
+      <c r="C6">
+        <v>1.37</v>
+      </c>
+      <c r="D6">
+        <v>2.46</v>
+      </c>
+      <c r="E6">
+        <v>3.49</v>
+      </c>
+      <c r="F6">
+        <v>3.09</v>
+      </c>
+      <c r="G6">
+        <v>2.97</v>
+      </c>
+      <c r="H6">
+        <v>3.78</v>
+      </c>
+      <c r="I6">
+        <v>4.13</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -427,7 +1052,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>16</v>
+        <v>160</v>
       </c>
       <c r="B3">
         <v>1.34</v>
@@ -441,7 +1066,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>32</v>
+        <v>320</v>
       </c>
       <c r="B4">
         <v>3.41</v>
@@ -455,7 +1080,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>48</v>
+        <v>480</v>
       </c>
       <c r="B5">
         <v>5.61</v>
@@ -469,7 +1094,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>64</v>
+        <v>640</v>
       </c>
       <c r="B6">
         <v>6.26</v>
@@ -483,7 +1108,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>80</v>
+        <v>800</v>
       </c>
       <c r="B7">
         <v>6.86</v>
@@ -497,13 +1122,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>96</v>
+        <v>960</v>
       </c>
       <c r="B8">
         <v>6.98</v>
       </c>
       <c r="C8">
-        <v>3.69</v>
+        <v>4.6900000000000004</v>
       </c>
       <c r="D8">
         <v>2.97</v>
@@ -511,13 +1136,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>112</v>
+        <v>1120</v>
       </c>
       <c r="B9">
         <v>9.25</v>
       </c>
       <c r="C9">
-        <v>4.5199999999999996</v>
+        <v>6.52</v>
       </c>
       <c r="D9">
         <v>3.78</v>
@@ -525,13 +1150,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>128</v>
+        <v>1280</v>
       </c>
       <c r="B10">
         <v>10</v>
       </c>
       <c r="C10">
-        <v>4.9400000000000004</v>
+        <v>6.94</v>
       </c>
       <c r="D10">
         <v>4.13</v>
@@ -546,27 +1171,307 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>160</v>
+      </c>
+      <c r="B3">
+        <v>1.34</v>
+      </c>
+      <c r="C3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D3">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>320</v>
+      </c>
+      <c r="B4">
+        <v>3.41</v>
+      </c>
+      <c r="C4">
+        <v>1.63</v>
+      </c>
+      <c r="D4">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>480</v>
+      </c>
+      <c r="B5">
+        <v>5.61</v>
+      </c>
+      <c r="C5">
+        <v>2.95</v>
+      </c>
+      <c r="D5">
+        <v>2.46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>640</v>
+      </c>
+      <c r="B6">
+        <v>6.26</v>
+      </c>
+      <c r="C6">
+        <v>4.18</v>
+      </c>
+      <c r="D6">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>800</v>
+      </c>
+      <c r="B7">
+        <v>6.86</v>
+      </c>
+      <c r="C7">
+        <v>3.73</v>
+      </c>
+      <c r="D7">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>960</v>
+      </c>
+      <c r="B8">
+        <v>6.98</v>
+      </c>
+      <c r="C8">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="D8">
+        <v>2.97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1120</v>
+      </c>
+      <c r="B9">
+        <v>9.25</v>
+      </c>
+      <c r="C9">
+        <v>6.52</v>
+      </c>
+      <c r="D9">
+        <v>3.78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1280</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>6.94</v>
+      </c>
+      <c r="D10">
+        <v>4.13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1814156-A872-4892-A765-58DB1AE6D2C6}">
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>160</v>
+      </c>
+      <c r="B3">
+        <v>1.34</v>
+      </c>
+      <c r="C3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D3">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>320</v>
+      </c>
+      <c r="B4">
+        <v>3.41</v>
+      </c>
+      <c r="C4">
+        <v>1.63</v>
+      </c>
+      <c r="D4">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>480</v>
+      </c>
+      <c r="B5">
+        <v>5.61</v>
+      </c>
+      <c r="C5">
+        <v>2.95</v>
+      </c>
+      <c r="D5">
+        <v>2.46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>640</v>
+      </c>
+      <c r="B6">
+        <v>6.26</v>
+      </c>
+      <c r="C6">
+        <v>4.18</v>
+      </c>
+      <c r="D6">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>800</v>
+      </c>
+      <c r="B7">
+        <v>6.86</v>
+      </c>
+      <c r="C7">
+        <v>3.73</v>
+      </c>
+      <c r="D7">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>960</v>
+      </c>
+      <c r="B8">
+        <v>6.98</v>
+      </c>
+      <c r="C8">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="D8">
+        <v>2.97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1120</v>
+      </c>
+      <c r="B9">
+        <v>9.25</v>
+      </c>
+      <c r="C9">
+        <v>6.52</v>
+      </c>
+      <c r="D9">
+        <v>3.78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1280</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>6.94</v>
+      </c>
+      <c r="D10">
+        <v>4.13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>